<commit_message>
update README && create class encode info
</commit_message>
<xml_diff>
--- a/design/detail_design.xlsx
+++ b/design/detail_design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19110" windowHeight="7575" activeTab="2"/>
+    <workbookView windowWidth="19110" windowHeight="7575"/>
   </bookViews>
   <sheets>
     <sheet name="main_function" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>SERVER</t>
   </si>
@@ -24,22 +24,70 @@
     <t>CLIENT</t>
   </si>
   <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>function</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>1{User}</t>
+  </si>
+  <si>
+    <t>"1"+user.toString()</t>
+  </si>
+  <si>
     <t>-handleLogin()</t>
   </si>
   <si>
     <t>-sendRequestFriend()</t>
   </si>
   <si>
+    <t>register</t>
+  </si>
+  <si>
+    <t>2{User}</t>
+  </si>
+  <si>
+    <t>"2"+user.toString()</t>
+  </si>
+  <si>
     <t>-handleRegister()</t>
   </si>
   <si>
     <t>-exceptRequestFriend()</t>
   </si>
   <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>3{Message}</t>
+  </si>
+  <si>
+    <t>"3"+message.toString()</t>
+  </si>
+  <si>
     <t>-receiveMessage()</t>
   </si>
   <si>
     <t>-searchUserByUsername()</t>
+  </si>
+  <si>
+    <t>search</t>
+  </si>
+  <si>
+    <t>4{key}</t>
+  </si>
+  <si>
+    <t>"4{\"key\":\""+key+"\"}"</t>
   </si>
   <si>
     <t>-sendMessage()</t>
@@ -59,10 +107,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -76,6 +124,29 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -89,13 +160,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -104,90 +168,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -211,6 +193,72 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -232,19 +280,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -256,168 +460,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -488,11 +536,65 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -512,41 +614,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -568,17 +642,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -590,144 +653,144 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -735,7 +798,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -757,40 +820,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
@@ -1121,121 +1160,184 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B3:F15"/>
+  <dimension ref="B2:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75"/>
   <cols>
     <col min="5" max="5" width="10.4" customWidth="1"/>
     <col min="6" max="6" width="11.5" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="11" max="11" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6">
+    <row r="2" ht="16.5"/>
+    <row r="3" spans="2:11">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="11"/>
+      <c r="F3" s="2"/>
+      <c r="H3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:11">
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="13"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="4"/>
+      <c r="H4" s="9">
+        <v>1</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="2:6">
-      <c r="B5" s="17" t="s">
+    <row r="5" spans="2:11">
+      <c r="B5" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="E5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="H5" s="9">
         <v>2</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="E5" s="18" t="s">
+      <c r="I5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11">
+      <c r="B6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="E6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="H6" s="9">
         <v>3</v>
       </c>
-      <c r="F5" s="13"/>
+      <c r="I6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="6" spans="2:6">
-      <c r="B6" s="19" t="s">
+    <row r="7" spans="2:11">
+      <c r="B7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="E7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="H7" s="9">
         <v>4</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="E6" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="13"/>
-    </row>
-    <row r="7" spans="2:6">
-      <c r="B7" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="E7" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="13"/>
+      <c r="I7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="2:6">
-      <c r="B8" s="20" t="s">
-        <v>8</v>
+      <c r="B8" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="E8" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="13"/>
+      <c r="E8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
-      <c r="E9" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="13"/>
+      <c r="E9" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
-      <c r="E10" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="13"/>
+      <c r="E10" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
-      <c r="E11" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="13"/>
+      <c r="E11" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="4"/>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="13"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="4"/>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="13"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="4"/>
     </row>
     <row r="15" ht="16.5" spans="2:6">
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="16"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1269,7 +1371,7 @@
   <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>

</xml_diff>